<commit_message>
Finished all questions and bonus.  Reviewed in class.
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volun\Documents\DA9\Excel\lookups_exercise-volunteercjt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EE94B3-E1F0-4987-B427-677CC6F83879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D55471-E17E-42C8-940E-D976673C0EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="91">
   <si>
     <t>Department</t>
   </si>
@@ -926,7 +926,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Arts Commission</c:v>
+              <c:v>Internal Audit</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1015,13 +1015,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3130600</c:v>
+                  <c:v>1382900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3652300</c:v>
+                  <c:v>1545700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3662400</c:v>
+                  <c:v>1525900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,13 +1080,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3115157.5599999898</c:v>
+                  <c:v>1250442.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3589693.2099999902</c:v>
+                  <c:v>1281335.23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3564983.04999999</c:v>
+                  <c:v>1393285.06</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2177,8 +2177,8 @@
   <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5258,7 +5258,7 @@
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="7" t="s">
         <v>90</v>
       </c>
     </row>
@@ -5463,6 +5463,9 @@
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="E63" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
@@ -5643,7 +5646,7 @@
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="15"/>
+        <f>_xlfn.XLOOKUP(A70,A7:A57,I7:I57,"not found",0)</f>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
@@ -5667,6 +5670,9 @@
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
+      <c r="E72" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
@@ -5889,11 +5895,11 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX(B$2:B$52,MATCH($A$87,$A$2:$A$52,0))</f>
-        <v>3130600</v>
+        <v>1382900</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX(C$2:C$52,MATCH($A$87,$A$2:$A$52,0))</f>
-        <v>3115157.5599999898</v>
+        <v>1250442.02</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -5902,11 +5908,11 @@
       </c>
       <c r="B85" s="6">
         <f>INDEX(G$2:G$52,MATCH($A$87,$A$2:$A$52,0))</f>
-        <v>3652300</v>
+        <v>1545700</v>
       </c>
       <c r="C85" s="6">
         <f>INDEX(H$2:H$52,MATCH($A$87,$A$2:$A$52,0))</f>
-        <v>3589693.2099999902</v>
+        <v>1281335.23</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -5915,16 +5921,16 @@
       </c>
       <c r="B86" s="6">
         <f>INDEX(L$2:L$52,MATCH($A$87,$A$2:$A$52,0))</f>
-        <v>3662400</v>
+        <v>1525900</v>
       </c>
       <c r="C86" s="6">
         <f>INDEX(M$2:M$52,MATCH($A$87,$A$2:$A$52,0))</f>
-        <v>3564983.04999999</v>
+        <v>1393285.06</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>